<commit_message>
doc: removes extrapolation explanation
</commit_message>
<xml_diff>
--- a/notebooks/experiment_tracker.xlsx
+++ b/notebooks/experiment_tracker.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -494,8 +494,94 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Random Forest with just a few hyperparameters performed a lot better than linear regression.
-It seems to be overfitting as we see validation scores much higher than training scores. It's a sign that would need to tune hyperparameters.</t>
+          <t>Random Forest with just a few hyperparameters performed just a little better than linear regression (validations score).
+It seems to be overfitting as we see validation scores much higher than training scores. It's a sign that tuning hyperparameters is needed.</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Random Forest with all expected features</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>To use as a baseline model with all features.</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Random Forest model with all features has decrease RSME and particularly in validation metrics.</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Random Forest with all features as categorical</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Changing temp and hum to categorical variables it will improve the model    specifically the prediction with boosting trees.</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Changing temp and hum into categorical variables did not improve the model. The expected improvement is for boosting models.</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Catboost</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Using all features as categorical variables it will perform better using boosting trees.</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Catboost model improved RSME compared to Random Forest (all cat vars) but not as good as Random Forest (temp/hum as numerical feat).</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>SVM Regressor</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>SVM Regressor can be a good model for this dataset as it is a linear model and extrapolates well.</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>SVM Regressor did not improve the model. Also a few features that it does not seem important on all models, now are, for example Working Day.
+This model will be discarded as it is not a good model for this dataset.</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>LightGBM</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Another boosting tree but lighter and known to be more accurate than Catboost.</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>LightGBM model did improve the model on Validation set. The gap between the validation and training set is not large as other models.</t>
         </is>
       </c>
     </row>
@@ -510,7 +596,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -573,7 +659,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>02/06/2022 19:39:40</t>
+          <t>05/06/2022 19:26:02</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -601,7 +687,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>02/06/2022 19:39:41</t>
+          <t>05/06/2022 19:26:03</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -633,7 +719,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>02/06/2022 19:39:43</t>
+          <t>05/06/2022 19:26:04</t>
         </is>
       </c>
       <c r="F4" t="inlineStr"/>
@@ -646,7 +732,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>['temp', 'rhum', 'wdsp', 'rain', 'holiday']</t>
+          <t>['temp_r', 'rhum', 'holiday', 'dayofweek', 'timesofday', 'wind_speed_group', 'rainfall_intensity', 'peak', 'working_day']</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -656,17 +742,17 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>[{ 'metric': RSME, 'train': 2.54,  'validation': 3.08, 'test': None }, { 'metric': MAE, 'train': 1.97,  'validation': 2.38, 'test': None }]</t>
+          <t>[{ 'metric': RSME, 'train': 2.25,  'validation': 2.70, 'test': None }, { 'metric': MAE, 'train': 1.67,  'validation': 2.00, 'test': None }]</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>02/06/2022 19:39:45</t>
+          <t>05/06/2022 19:26:06</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Added holiday as a predictor</t>
+          <t>Added all predictors and using preprocessing</t>
         </is>
       </c>
     </row>
@@ -678,66 +764,66 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>['temp', 'rhum', 'wdsp', 'rain', 'holiday', 'dayofweek_n']</t>
+          <t>['temp_bin', 'rhum_bin', 'holiday', 'dayofweek', 'timesofday', 'wind_speed_group', 'rainfall_intensity', 'peak', 'working_day']</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>{'bootstrap': True, 'ccp_alpha': 0.0, 'criterion': 'squared_error', 'max_depth': 10, 'max_features': 'auto', 'max_leaf_nodes': None, 'max_samples': None, 'min_impurity_decrease': 0.0, 'min_samples_leaf': 1, 'min_samples_split': 2, 'min_weight_fraction_leaf': 0.0, 'n_estimators': 100, 'n_jobs': None, 'oob_score': False, 'random_state': 42, 'verbose': 0, 'warm_start': False}</t>
+          <t>{'bootstrap': True, 'ccp_alpha': 0.0, 'criterion': 'squared_error', 'max_depth': 20, 'max_features': 'auto', 'max_leaf_nodes': None, 'max_samples': None, 'min_impurity_decrease': 0.0, 'min_samples_leaf': 1, 'min_samples_split': 5, 'min_weight_fraction_leaf': 0.0, 'n_estimators': 100, 'n_jobs': -1, 'oob_score': False, 'random_state': 0, 'verbose': 0, 'warm_start': False}</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>[{ 'metric': RSME, 'train': 2.44,  'validation': 3.03, 'test': None }, { 'metric': MAE, 'train': 1.90,  'validation': 2.35, 'test': None }]</t>
+          <t>[{ 'metric': RSME, 'train': 2.10,  'validation': 2.81, 'test': None }, { 'metric': MAE, 'train': 1.53,  'validation': 2.09, 'test': None }]</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>02/06/2022 19:39:46</t>
+          <t>05/06/2022 19:26:19</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Added holiday + dayofweek as a predictor</t>
+          <t>Added all predictors and using preprocessing</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Random Forest</t>
+          <t>Catboost model</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>['temp_r', 'rhum', 'holiday', 'dayofweek', 'timesofday', 'wind_speed_group', 'rainfall_intensity', 'peak', 'working_day']</t>
+          <t>['temp_bin', 'rhum_bin', 'holiday', 'dayofweek', 'timesofday', 'wind_speed_group', 'rainfall_intensity', 'peak', 'working_day']</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>{'bootstrap': True, 'ccp_alpha': 0.0, 'criterion': 'squared_error', 'max_depth': 20, 'max_features': 'auto', 'max_leaf_nodes': None, 'max_samples': None, 'min_impurity_decrease': 0.0, 'min_samples_leaf': 1, 'min_samples_split': 5, 'min_weight_fraction_leaf': 0.0, 'n_estimators': 100, 'n_jobs': -1, 'oob_score': False, 'random_state': 0, 'verbose': 0, 'warm_start': False}</t>
+          <t>{'loss_function': 'RMSE', 'verbose': 25, 'n_estimators': 100, 'random_state': 42}</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>[{ 'metric': RSME, 'train': 1.63,  'validation': 2.77, 'test': None }, { 'metric': MAE, 'train': 1.19,  'validation': 2.06, 'test': None }]</t>
+          <t>[{ 'metric': RSME, 'train': 2.48,  'validation': 2.70, 'test': None }, { 'metric': MAE, 'train': 1.83,  'validation': 2.00, 'test': None }]</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>02/06/2022 19:39:49</t>
+          <t>05/06/2022 19:26:26</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Added all predictors and using preprocessing</t>
+          <t>Added all categoricals features to use Catboost model.</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Random Forest</t>
+          <t>Support Vector Regression</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -747,29 +833,25 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>{'bootstrap': True, 'ccp_alpha': 0.0, 'criterion': 'squared_error', 'max_depth': 20, 'max_features': 'auto', 'max_leaf_nodes': None, 'max_samples': None, 'min_impurity_decrease': 0.0, 'min_samples_leaf': 1, 'min_samples_split': 5, 'min_weight_fraction_leaf': 0.0, 'n_estimators': 100, 'n_jobs': -1, 'oob_score': False, 'random_state': 0, 'verbose': 0, 'warm_start': False}</t>
+          <t>{'C': 100, 'cache_size': 200, 'coef0': 0.0, 'degree': 5, 'epsilon': 0.1, 'gamma': 'scale', 'kernel': 'poly', 'max_iter': -1, 'shrinking': True, 'tol': 0.001, 'verbose': False}</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>[{ 'metric': RSME, 'train': 2.10,  'validation': 2.81, 'test': None }, { 'metric': MAE, 'train': 1.53,  'validation': 2.09, 'test': None }]</t>
+          <t>[{ 'metric': RSME, 'train': 2.73,  'validation': 2.87, 'test': None }, { 'metric': MAE, 'train': 1.82,  'validation': 2.03, 'test': None }]</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>02/06/2022 19:40:10</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>Added all predictors and using preprocessing</t>
-        </is>
-      </c>
+          <t>05/06/2022 19:27:48</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Catboost model</t>
+          <t>LightGBM</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -779,304 +861,20 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>{'learning_rate': 0.1, 'depth': 8, 'loss_function': 'RMSE', 'verbose': 250, 'n_estimators': 1500, 'random_state': 0, 'early_stopping_rounds': 10}</t>
+          <t>{'boosting_type': 'gbdt', 'class_weight': None, 'colsample_bytree': 1.0, 'importance_type': 'split', 'learning_rate': 0.1, 'max_depth': -1, 'min_child_samples': 20, 'min_child_weight': 0.001, 'min_split_gain': 0.0, 'n_estimators': 100, 'n_jobs': -1, 'num_leaves': 31, 'objective': None, 'random_state': 42, 'reg_alpha': 0.0, 'reg_lambda': 0.0, 'silent': True, 'subsample': 1.0, 'subsample_for_bin': 200000, 'subsample_freq': 0, 'metric': 'rmse', 'verbose': 25}</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>[{ 'metric': RSME, 'train': 2.00,  'validation': 2.93, 'test': None }, { 'metric': MAE, 'train': 1.40,  'validation': 2.17, 'test': None }]</t>
+          <t>[{ 'metric': RSME, 'train': 2.51,  'validation': 2.68, 'test': None }, { 'metric': MAE, 'train': 1.86,  'validation': 1.99, 'test': None }]</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>02/06/2022 19:40:25</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>Added all categoricals features to use Catboost model.</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Support Vector Regression</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>['temp_bin', 'rhum_bin', 'holiday', 'dayofweek', 'timesofday', 'wind_speed_group', 'rainfall_intensity', 'peak', 'working_day']</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>{'C': 100, 'cache_size': 200, 'coef0': 0.0, 'degree': 3, 'epsilon': 0.1, 'gamma': 'scale', 'kernel': 'poly', 'max_iter': -1, 'shrinking': True, 'tol': 0.001, 'verbose': False}</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>[{ 'metric': RSME, 'train': 2.75,  'validation': 2.78, 'test': None }, { 'metric': MAE, 'train': 1.89,  'validation': 1.96, 'test': None }]</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>02/06/2022 19:44:51</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Support Vector Regression</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>['temp_bin', 'rhum_bin', 'holiday', 'dayofweek', 'timesofday', 'wind_speed_group', 'rainfall_intensity', 'peak', 'working_day']</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>{'C': 100, 'cache_size': 200, 'coef0': 0.0, 'degree': 3, 'epsilon': 0.1, 'gamma': 'scale', 'kernel': 'poly', 'max_iter': 100, 'shrinking': True, 'tol': 0.001, 'verbose': False}</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>[{ 'metric': RSME, 'train': 9.54,  'validation': 9.59, 'test': None }, { 'metric': MAE, 'train': 7.86,  'validation': 7.84, 'test': None }]</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>02/06/2022 19:47:59</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr"/>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Support Vector Regression</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>['temp_bin', 'rhum_bin', 'holiday', 'dayofweek', 'timesofday', 'wind_speed_group', 'rainfall_intensity', 'peak', 'working_day']</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>{'C': 100, 'cache_size': 200, 'coef0': 0.0, 'degree': 3, 'epsilon': 0.1, 'gamma': 'scale', 'kernel': 'poly', 'max_iter': 1000, 'shrinking': True, 'tol': 0.001, 'verbose': False}</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>[{ 'metric': RSME, 'train': 5.15,  'validation': 5.17, 'test': None }, { 'metric': MAE, 'train': 3.97,  'validation': 4.04, 'test': None }]</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>02/06/2022 19:48:47</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Support Vector Regression</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>['temp_bin', 'rhum_bin', 'holiday', 'dayofweek', 'timesofday', 'wind_speed_group', 'rainfall_intensity', 'peak', 'working_day']</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>{'C': 100, 'cache_size': 200, 'coef0': 0.0, 'degree': 3, 'epsilon': 0.1, 'gamma': 'scale', 'kernel': 'poly', 'max_iter': -1, 'shrinking': True, 'tol': 0.001, 'verbose': False}</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>[{ 'metric': RSME, 'train': 2.75,  'validation': 2.78, 'test': None }, { 'metric': MAE, 'train': 1.89,  'validation': 1.96, 'test': None }]</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>02/06/2022 19:50:23</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr"/>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Support Vector Regression</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>['temp_bin', 'rhum_bin', 'holiday', 'dayofweek', 'timesofday', 'wind_speed_group', 'rainfall_intensity', 'peak', 'working_day']</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>{'C': 100, 'cache_size': 200, 'coef0': 0.0, 'degree': 5, 'epsilon': 0.1, 'gamma': 'scale', 'kernel': 'poly', 'max_iter': -1, 'shrinking': True, 'tol': 0.001, 'verbose': False}</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>[{ 'metric': RSME, 'train': 2.73,  'validation': 2.87, 'test': None }, { 'metric': MAE, 'train': 1.82,  'validation': 2.03, 'test': None }]</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>02/06/2022 19:52:48</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr"/>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>LightGBM</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>['temp_bin', 'rhum_bin', 'holiday', 'dayofweek', 'timesofday', 'wind_speed_group', 'rainfall_intensity', 'peak', 'working_day']</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>{'boosting_type': 'gbdt', 'class_weight': None, 'colsample_bytree': 1.0, 'importance_type': 'split', 'learning_rate': 0.01, 'max_depth': 15, 'min_child_samples': 20, 'min_child_weight': 0.001, 'min_split_gain': 0.0, 'n_estimators': 1000, 'n_jobs': 2, 'num_leaves': 30, 'objective': None, 'random_state': 0, 'reg_alpha': 0.0, 'reg_lambda': 0.0, 'silent': True, 'subsample': 0.7, 'subsample_for_bin': 200000, 'subsample_freq': 0, 'metric': 'rmse'}</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>[{ 'metric': RSME, 'train': 2.52,  'validation': 2.68, 'test': None }, { 'metric': MAE, 'train': 1.87,  'validation': 1.99, 'test': None }]</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>02/06/2022 20:27:27</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr"/>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>LightGBM</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>['temp_bin', 'rhum_bin', 'holiday', 'dayofweek', 'timesofday', 'wind_speed_group', 'rainfall_intensity', 'peak', 'working_day']</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>{'boosting_type': 'gbdt', 'class_weight': None, 'colsample_bytree': 1.0, 'importance_type': 'split', 'learning_rate': 0.001, 'max_depth': 15, 'min_child_samples': 20, 'min_child_weight': 0.001, 'min_split_gain': 0.0, 'n_estimators': 1000, 'n_jobs': 2, 'num_leaves': 30, 'objective': None, 'random_state': 0, 'reg_alpha': 0.0, 'reg_lambda': 0.0, 'silent': True, 'subsample': 0.7, 'subsample_for_bin': 200000, 'subsample_freq': 0, 'metric': 'rmse'}</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>[{ 'metric': RSME, 'train': 2.86,  'validation': 2.86, 'test': None }, { 'metric': MAE, 'train': 2.20,  'validation': 2.21, 'test': None }]</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>02/06/2022 20:27:47</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr"/>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>LightGBM</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>['temp_bin', 'rhum_bin', 'holiday', 'dayofweek', 'timesofday', 'wind_speed_group', 'rainfall_intensity', 'peak', 'working_day']</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>{'boosting_type': 'gbdt', 'class_weight': None, 'colsample_bytree': 1.0, 'importance_type': 'split', 'learning_rate': 0.001, 'max_depth': 15, 'min_child_samples': 20, 'min_child_weight': 0.001, 'min_split_gain': 0.0, 'n_estimators': 1000, 'n_jobs': 2, 'num_leaves': 30, 'objective': None, 'random_state': 0, 'reg_alpha': 0.0, 'reg_lambda': 0.0, 'silent': True, 'subsample': 0.7, 'subsample_for_bin': 200000, 'subsample_freq': 0, 'metric': 'rmse', 'verbosity': 100}</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>[{ 'metric': RSME, 'train': 2.86,  'validation': 2.86, 'test': None }, { 'metric': MAE, 'train': 2.20,  'validation': 2.21, 'test': None }]</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>02/06/2022 20:28:53</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr"/>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>LightGBM</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>['temp_bin', 'rhum_bin', 'holiday', 'dayofweek', 'timesofday', 'wind_speed_group', 'rainfall_intensity', 'peak', 'working_day']</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>{'boosting_type': 'gbdt', 'class_weight': None, 'colsample_bytree': 1.0, 'importance_type': 'split', 'learning_rate': 0.001, 'max_depth': 15, 'min_child_samples': 20, 'min_child_weight': 0.001, 'min_split_gain': 0.0, 'n_estimators': 1000, 'n_jobs': 2, 'num_leaves': 30, 'objective': None, 'random_state': 0, 'reg_alpha': 0.0, 'reg_lambda': 0.0, 'silent': True, 'subsample': 0.7, 'subsample_for_bin': 200000, 'subsample_freq': 0, 'metric': 'rmse'}</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>[{ 'metric': RSME, 'train': 2.86,  'validation': 2.86, 'test': None }, { 'metric': MAE, 'train': 2.20,  'validation': 2.21, 'test': None }]</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>02/06/2022 20:29:40</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr"/>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>LightGBM</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>['temp_bin', 'rhum_bin', 'holiday', 'dayofweek', 'timesofday', 'wind_speed_group', 'rainfall_intensity', 'peak', 'working_day']</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>{'boosting_type': 'gbdt', 'class_weight': None, 'colsample_bytree': 1.0, 'importance_type': 'split', 'learning_rate': 0.01, 'max_depth': 15, 'min_child_samples': 20, 'min_child_weight': 0.001, 'min_split_gain': 0.0, 'n_estimators': 10000, 'n_jobs': 2, 'num_leaves': 30, 'objective': None, 'random_state': 0, 'reg_alpha': 0.0, 'reg_lambda': 0.0, 'silent': True, 'subsample': 0.7, 'subsample_for_bin': 200000, 'subsample_freq': 0, 'metric': 'rmse'}</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>[{ 'metric': RSME, 'train': 2.18,  'validation': 2.82, 'test': None }, { 'metric': MAE, 'train': 1.60,  'validation': 2.10, 'test': None }]</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>02/06/2022 20:30:13</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr"/>
+          <t>05/06/2022 19:28:35</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
feat: new method to print partial experiments with its metrics
</commit_message>
<xml_diff>
--- a/notebooks/experiment_tracker.xlsx
+++ b/notebooks/experiment_tracker.xlsx
@@ -659,7 +659,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>05/06/2022 19:26:02</t>
+          <t>07/06/2022 21:13:44</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -687,7 +687,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>05/06/2022 19:26:03</t>
+          <t>07/06/2022 21:13:45</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -719,7 +719,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>05/06/2022 19:26:04</t>
+          <t>07/06/2022 21:13:46</t>
         </is>
       </c>
       <c r="F4" t="inlineStr"/>
@@ -747,7 +747,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>05/06/2022 19:26:06</t>
+          <t>07/06/2022 21:13:48</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -779,7 +779,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>05/06/2022 19:26:19</t>
+          <t>07/06/2022 21:13:59</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -811,7 +811,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>05/06/2022 19:26:26</t>
+          <t>07/06/2022 21:14:05</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -843,7 +843,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>05/06/2022 19:27:48</t>
+          <t>07/06/2022 21:15:31</t>
         </is>
       </c>
       <c r="F8" t="inlineStr"/>
@@ -871,7 +871,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>05/06/2022 19:28:35</t>
+          <t>07/06/2022 21:16:25</t>
         </is>
       </c>
       <c r="F9" t="inlineStr"/>

</xml_diff>